<commit_message>
documentation and making email body html
</commit_message>
<xml_diff>
--- a/batches/01.xlsx
+++ b/batches/01.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janindu Laknath\Desktop\mail merge\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janindu Laknath\Desktop\CLI AUTOMATION\batches\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C3C398E-B48B-47DF-BDDE-9C6311CC8859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{525B3312-D65F-4DFC-901E-13BA7DF09BF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28800" yWindow="-4560" windowWidth="14400" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -398,7 +398,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>